<commit_message>
Updated Task reminder proj. with proper comments
</commit_message>
<xml_diff>
--- a/Task_Reminder/ReminderDiary.xlsx
+++ b/Task_Reminder/ReminderDiary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github Projects\Basic-Python-Projects\Task_Reminder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFB8FFD-725B-4887-9457-893D97074CAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732D3A37-C662-4D7C-BDD4-59B7E427F26B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{212DFD29-CF70-444E-868B-3750A8C4E099}"/>
+    <workbookView xWindow="4080" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{212DFD29-CF70-444E-868B-3750A8C4E099}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -437,7 +437,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>0.42638888888888887</v>
+        <v>0.28125</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -448,7 +448,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>0.42708333333333331</v>
+        <v>0.28263888888888888</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>

</xml_diff>